<commit_message>
find info -> any
</commit_message>
<xml_diff>
--- a/OOPproject4/car_info.xlsx
+++ b/OOPproject4/car_info.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="14850" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2190" yWindow="2610" windowWidth="22650" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="car_info" sheetId="1" state="visible" r:id="rId1"/>
@@ -444,10 +444,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5" outlineLevelCol="0"/>
@@ -485,63 +485,243 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="n"/>
-      <c r="B2" s="0" t="n"/>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:37:54</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>245우9315</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n"/>
-      <c r="B3" s="0" t="n"/>
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:37:54</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>65노0887</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n"/>
-      <c r="B4" s="0" t="n"/>
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:37:54</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>1234568</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="n"/>
-      <c r="B5" s="0" t="n"/>
-      <c r="E5" s="0" t="n"/>
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:45:47</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>245우9315</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>101동</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>102호</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>김철수</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="n"/>
-      <c r="B6" s="0" t="n"/>
-      <c r="E6" s="0" t="n"/>
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:45:47</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>홍길동</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="n"/>
-      <c r="B7" s="0" t="n"/>
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:45:47</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>1234568</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="0" t="n"/>
-      <c r="B8" s="0" t="n"/>
-      <c r="E8" s="0" t="n"/>
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:46:10</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>245우9315</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>101동</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>102호</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>김철수</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="0" t="n"/>
-      <c r="B9" s="0" t="n"/>
-      <c r="E9" s="0" t="n"/>
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:46:10</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>홍길동</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="0" t="n"/>
-      <c r="B10" s="0" t="n"/>
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:46:10</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>1234568</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="0" t="n"/>
-      <c r="B11" s="0" t="n"/>
-      <c r="E11" s="0" t="n"/>
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:46:43</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>245우9315</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>101동</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>102호</t>
+        </is>
+      </c>
+      <c r="E11" s="0" t="inlineStr">
+        <is>
+          <t>김철수</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="0" t="n"/>
-      <c r="B12" s="0" t="n"/>
-      <c r="E12" s="0" t="n"/>
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:46:43</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E12" s="0" t="inlineStr">
+        <is>
+          <t>홍길동</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="0" t="n"/>
-      <c r="B13" s="0" t="n"/>
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-05 21:46:43</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>1234568</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>2022-12-06 12:48:13</t>
+          <t>2022-12-07 20:12:33</t>
         </is>
       </c>
       <c r="B14" s="0" t="inlineStr">
@@ -568,7 +748,7 @@
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>2022-12-06 12:48:13</t>
+          <t>2022-12-07 20:12:33</t>
         </is>
       </c>
       <c r="B15" s="0" t="inlineStr">
@@ -595,7 +775,7 @@
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>2022-12-06 12:48:13</t>
+          <t>2022-12-07 20:12:33</t>
         </is>
       </c>
       <c r="B16" s="0" t="inlineStr">
@@ -605,68 +785,542 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2022-12-06 21:30:10</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 20:20:31</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>245우9315</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>101동</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>102호</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E17" s="0" t="inlineStr">
         <is>
           <t>김철수</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2022-12-06 21:30:10</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 20:20:31</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>65노0887</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>103동</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="0" t="inlineStr">
         <is>
           <t>1902호</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E18" s="0" t="inlineStr">
         <is>
           <t>홍길동</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2022-12-06 21:30:10</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 20:20:31</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>1234568</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 22:59:51</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>245우9315</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>101동</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>102호</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>김철수</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 22:59:51</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>홍길동</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 22:59:51</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>1234568</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:04:57</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>245우9315</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>101동</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>102호</t>
+        </is>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>김철수</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:04:57</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
+        <is>
+          <t>홍길동</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:04:57</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>1234568</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:29:27</t>
+        </is>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>245우9315</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>101동</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>102호</t>
+        </is>
+      </c>
+      <c r="E26" s="0" t="inlineStr">
+        <is>
+          <t>김철수</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:29:27</t>
+        </is>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E27" s="0" t="inlineStr">
+        <is>
+          <t>홍길동</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:29:27</t>
+        </is>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>1234568</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:29:27</t>
+        </is>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>245낱9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:29:27</t>
+        </is>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>245깁9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:29:27</t>
+        </is>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>247가9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:30:15</t>
+        </is>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>245우9315</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>101동</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>102호</t>
+        </is>
+      </c>
+      <c r="E32" s="0" t="inlineStr">
+        <is>
+          <t>김철수</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:30:15</t>
+        </is>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E33" s="0" t="inlineStr">
+        <is>
+          <t>홍길동</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:30:15</t>
+        </is>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>1234568</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:30:15</t>
+        </is>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>245낱9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:30:15</t>
+        </is>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>245깁9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="inlineStr">
+        <is>
+          <t>2022-12-07 23:30:15</t>
+        </is>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>247가9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2022-12-08 00:04:08</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>245우9315</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>101동</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>102호</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>김철수</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2022-12-08 00:04:08</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>747가9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2022-12-08 00:04:08</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>홍길동</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2022-12-08 00:04:08</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>1234568</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2022-12-08 00:04:08</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>747가9317</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2022-12-08 00:04:08</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>245낱9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2022-12-08 00:04:08</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>245깁9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2022-12-08 00:04:08</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>247가9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2022-12-08 00:04:08</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>245가9315</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed to dynamic query
</commit_message>
<xml_diff>
--- a/OOPproject4/car_info.xlsx
+++ b/OOPproject4/car_info.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2190" yWindow="2610" windowWidth="22650" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="14850" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="car_info" sheetId="1" state="visible" r:id="rId1"/>
@@ -56,7 +56,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -67,6 +67,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -444,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
@@ -721,7 +722,7 @@
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 20:12:33</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B14" s="0" t="inlineStr">
@@ -748,178 +749,148 @@
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 20:12:33</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>65노0887</t>
+          <t>747가9315</t>
         </is>
       </c>
       <c r="C15" s="0" t="inlineStr">
         <is>
-          <t>103동</t>
+          <t>102동</t>
         </is>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>1902호</t>
+          <t>204호</t>
         </is>
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>홍길동</t>
+          <t>진도진</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 20:12:33</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>1234568</t>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t>홍길동</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 20:20:31</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>245우9315</t>
-        </is>
-      </c>
-      <c r="C17" s="0" t="inlineStr">
-        <is>
-          <t>101동</t>
-        </is>
-      </c>
-      <c r="D17" s="0" t="inlineStr">
-        <is>
-          <t>102호</t>
-        </is>
-      </c>
-      <c r="E17" s="0" t="inlineStr">
-        <is>
-          <t>김철수</t>
+          <t>1234568</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 20:20:31</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>65노0887</t>
+          <t>747가9317</t>
         </is>
       </c>
       <c r="C18" s="0" t="inlineStr">
         <is>
-          <t>103동</t>
+          <t>105동</t>
         </is>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>1902호</t>
+          <t>1201호</t>
         </is>
       </c>
       <c r="E18" s="0" t="inlineStr">
         <is>
-          <t>홍길동</t>
+          <t>손흥민</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 20:20:31</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>1234568</t>
+          <t>245낱9315</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 22:59:51</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>245우9315</t>
-        </is>
-      </c>
-      <c r="C20" s="0" t="inlineStr">
-        <is>
-          <t>101동</t>
-        </is>
-      </c>
-      <c r="D20" s="0" t="inlineStr">
-        <is>
-          <t>102호</t>
-        </is>
-      </c>
-      <c r="E20" s="0" t="inlineStr">
-        <is>
-          <t>김철수</t>
+          <t>245깁9315</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 22:59:51</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>65노0887</t>
-        </is>
-      </c>
-      <c r="C21" s="0" t="inlineStr">
-        <is>
-          <t>103동</t>
-        </is>
-      </c>
-      <c r="D21" s="0" t="inlineStr">
-        <is>
-          <t>1902호</t>
-        </is>
-      </c>
-      <c r="E21" s="0" t="inlineStr">
-        <is>
-          <t>홍길동</t>
+          <t>247가9315</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 22:59:51</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>1234568</t>
+          <t>245가9315</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 23:04:57</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B23" s="0" t="inlineStr">
@@ -946,379 +917,475 @@
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 23:04:57</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>65노0887</t>
+          <t>747가9315</t>
         </is>
       </c>
       <c r="C24" s="0" t="inlineStr">
         <is>
-          <t>103동</t>
+          <t>102동</t>
         </is>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>1902호</t>
+          <t>204호</t>
         </is>
       </c>
       <c r="E24" s="0" t="inlineStr">
         <is>
-          <t>홍길동</t>
+          <t>진도진</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 23:04:57</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>1234568</t>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E25" s="0" t="inlineStr">
+        <is>
+          <t>홍길동</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 23:29:27</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>245우9315</t>
-        </is>
-      </c>
-      <c r="C26" s="0" t="inlineStr">
-        <is>
-          <t>101동</t>
-        </is>
-      </c>
-      <c r="D26" s="0" t="inlineStr">
-        <is>
-          <t>102호</t>
-        </is>
-      </c>
-      <c r="E26" s="0" t="inlineStr">
-        <is>
-          <t>김철수</t>
+          <t>1234568</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 23:29:27</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>65노0887</t>
+          <t>747가9317</t>
         </is>
       </c>
       <c r="C27" s="0" t="inlineStr">
         <is>
-          <t>103동</t>
+          <t>105동</t>
         </is>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>1902호</t>
+          <t>1201호</t>
         </is>
       </c>
       <c r="E27" s="0" t="inlineStr">
         <is>
-          <t>홍길동</t>
+          <t>손흥민</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 23:29:27</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>1234568</t>
+          <t>245낱9315</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 23:29:27</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>245낱9315</t>
+          <t>245깁9315</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 23:29:27</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>245깁9315</t>
+          <t>247가9315</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>2022-12-07 23:29:27</t>
+          <t>2022-12-09 15:38:10</t>
         </is>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>247가9315</t>
+          <t>245가9315</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="0" t="inlineStr">
-        <is>
-          <t>2022-12-07 23:30:15</t>
-        </is>
-      </c>
-      <c r="B32" s="0" t="inlineStr">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2022-12-09 15:39:48</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>245우9315</t>
         </is>
       </c>
-      <c r="C32" s="0" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>101동</t>
         </is>
       </c>
-      <c r="D32" s="0" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>102호</t>
         </is>
       </c>
-      <c r="E32" s="0" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>김철수</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="0" t="inlineStr">
-        <is>
-          <t>2022-12-07 23:30:15</t>
-        </is>
-      </c>
-      <c r="B33" s="0" t="inlineStr">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2022-12-09 15:39:48</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>747가9315</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>102동</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>204호</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>진도진</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2022-12-09 15:39:48</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>65노0887</t>
         </is>
       </c>
-      <c r="C33" s="0" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>103동</t>
         </is>
       </c>
-      <c r="D33" s="0" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>1902호</t>
         </is>
       </c>
-      <c r="E33" s="0" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>홍길동</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="0" t="inlineStr">
-        <is>
-          <t>2022-12-07 23:30:15</t>
-        </is>
-      </c>
-      <c r="B34" s="0" t="inlineStr">
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2022-12-09 15:39:48</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>1234568</t>
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="0" t="inlineStr">
-        <is>
-          <t>2022-12-07 23:30:15</t>
-        </is>
-      </c>
-      <c r="B35" s="0" t="inlineStr">
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2022-12-09 15:39:48</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>747가9317</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>105동</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>1201호</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>손흥민</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2022-12-09 15:39:48</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>245낱9315</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="0" t="inlineStr">
-        <is>
-          <t>2022-12-07 23:30:15</t>
-        </is>
-      </c>
-      <c r="B36" s="0" t="inlineStr">
-        <is>
-          <t>245깁9315</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="0" t="inlineStr">
-        <is>
-          <t>2022-12-07 23:30:15</t>
-        </is>
-      </c>
-      <c r="B37" s="0" t="inlineStr">
-        <is>
-          <t>247가9315</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2022-12-08 00:04:08</t>
+          <t>2022-12-09 15:39:48</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>245우9315</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>101동</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>102호</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>김철수</t>
+          <t>245깁9315</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2022-12-08 00:04:08</t>
+          <t>2022-12-09 15:39:48</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>747가9315</t>
+          <t>247가9315</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2022-12-08 00:04:08</t>
+          <t>2022-12-09 15:39:48</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>65노0887</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>103동</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>1902호</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>홍길동</t>
+          <t>245가9315</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2022-12-08 00:04:08</t>
+          <t>2022-12-09 15:39:48</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1234568</t>
+          <t>245우9315</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>101동</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>102호</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>김철수</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2022-12-08 00:04:08</t>
+          <t>2022-12-09 15:39:48</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>747가9317</t>
+          <t>747가9315</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>102동</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>204호</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>진도진</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2022-12-08 00:04:08</t>
+          <t>2022-12-09 15:39:48</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>245낱9315</t>
+          <t>65노0887</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>103동</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>1902호</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>홍길동</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2022-12-08 00:04:08</t>
+          <t>2022-12-09 15:39:48</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>245깁9315</t>
+          <t>1234568</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2022-12-08 00:04:08</t>
+          <t>2022-12-09 15:39:48</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>247가9315</t>
+          <t>747가9317</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>105동</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>1201호</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>손흥민</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2022-12-08 00:04:08</t>
+          <t>2022-12-09 15:39:48</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
+        <is>
+          <t>245낱9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2022-12-09 15:39:48</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>245깁9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2022-12-09 15:39:48</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>247가9315</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2022-12-09 15:39:48</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>245가9315</t>
         </is>
@@ -1335,10 +1402,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5" outlineLevelCol="0"/>
@@ -1440,6 +1507,186 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>44896</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>14너4912</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>타이칸</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>129동</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>1403호</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>송중기</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>44565</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>747가9315</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>그랜져</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>102동</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>204호</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>진도진</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>44291</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>123가4568</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>레이</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>104동</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>1001호</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>진양철</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>44683</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>747가9317</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>모닝</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>105동</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>1201호</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>손흥민</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>44672</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>245날9315</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>스포티지</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>104동</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>903호</t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>황희찬</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>44886</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>245김9315</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>카니발</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>102동</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>402호</t>
+        </is>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>이강인</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>